<commit_message>
Added admin view of quote request controller. No security or login implemented yet, though.
</commit_message>
<xml_diff>
--- a/doc/Dermbids Feature List.xlsx
+++ b/doc/Dermbids Feature List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19020" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19020" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Background" sheetId="2" r:id="rId1"/>
@@ -2806,6 +2806,96 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="TextBox 41"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="104775" y="18830925"/>
+          <a:ext cx="11515725" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>States that a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> quote request could be in:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>1. New - the request was just submitted and needs to be reviewed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>2. Active - the request is in processing, awaiting the feedback necessary to complete a quote</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>3. Archived - the quote requests have been sent</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3295,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A42:I45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3340,9 +3430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>